<commit_message>
FIX #0 ajout des variables de langue pour le service initiateur
</commit_message>
<xml_diff>
--- a/modules/templates/templates/styles/office/spreadsheet.xlsx
+++ b/modules/templates/templates/styles/office/spreadsheet.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" state="visible" r:id="rId2"/>
@@ -13,418 +13,459 @@
     <sheet name="Feuil3" sheetId="3" state="visible" r:id="rId4"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
+  <extLst>
+    <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
+      <loext:extCalcPr stringRefSyntax="CalcA1ExcelA1"/>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="141" uniqueCount="136">
-  <si>
-    <t>TITLE</t>
-  </si>
-  <si>
-    <t>TAG</t>
-  </si>
-  <si>
-    <t>VAR</t>
-  </si>
-  <si>
-    <t>Contact externe : Type de contact</t>
-  </si>
-  <si>
-    <t>contact.contact_type_label</t>
-  </si>
-  <si>
-    <t>[contact.contact_type_label]</t>
-  </si>
-  <si>
-    <t>Contact externe : Structure</t>
-  </si>
-  <si>
-    <t>contact.society</t>
-  </si>
-  <si>
-    <t>[contact.society]</t>
-  </si>
-  <si>
-    <t>Contact externe : Sigle de la structure</t>
-  </si>
-  <si>
-    <t>contact.society_short</t>
-  </si>
-  <si>
-    <t>[contact.society_short]</t>
-  </si>
-  <si>
-    <t>Contact externes : nom du contact</t>
-  </si>
-  <si>
-    <t>contact.contact_lastname</t>
-  </si>
-  <si>
-    <t>[contact.contact_lastname]</t>
-  </si>
-  <si>
-    <t>Contact externes : prénom du contact</t>
-  </si>
-  <si>
-    <t>contact.contact_firstname</t>
-  </si>
-  <si>
-    <t>[contact.contact_firstname]</t>
-  </si>
-  <si>
-    <t>Contact externe : Adresse Dénomination</t>
-  </si>
-  <si>
-    <t>contact.contact_purpose_label</t>
-  </si>
-  <si>
-    <t>[contact.contact_purpose_label]</t>
-  </si>
-  <si>
-    <t>Contact externe : Adresse Service</t>
-  </si>
-  <si>
-    <t>contact.departement</t>
-  </si>
-  <si>
-    <t>[contact.departement]</t>
-  </si>
-  <si>
-    <t>Contact externe : Adresse Civilité</t>
-  </si>
-  <si>
-    <t>contact.title</t>
-  </si>
-  <si>
-    <t>[contact.title]</t>
-  </si>
-  <si>
-    <t>Contact externe : Adresse Nom</t>
-  </si>
-  <si>
-    <t>contact.lastname</t>
-  </si>
-  <si>
-    <t>[contact.lastname]</t>
-  </si>
-  <si>
-    <t>Contact externe : Adresse Prénom</t>
-  </si>
-  <si>
-    <t>contact.firstname</t>
-  </si>
-  <si>
-    <t>[contact.firstname]</t>
-  </si>
-  <si>
-    <t>Contact externe : Adresse Fonction</t>
-  </si>
-  <si>
-    <t>contact.function</t>
-  </si>
-  <si>
-    <t>[contact.function]</t>
-  </si>
-  <si>
-    <t>Contact externe : Adresse Etage, bureau, porte</t>
-  </si>
-  <si>
-    <t>contact.occupancy</t>
-  </si>
-  <si>
-    <t>[contact.occupancy]</t>
-  </si>
-  <si>
-    <t>Contact externe : Adresse N°</t>
-  </si>
-  <si>
-    <t>contact.address_num</t>
-  </si>
-  <si>
-    <t>[contact.address_num]</t>
-  </si>
-  <si>
-    <t>Contact externe : Adresse Rue</t>
-  </si>
-  <si>
-    <t>contact.address_street</t>
-  </si>
-  <si>
-    <t>[contact.address_street]</t>
-  </si>
-  <si>
-    <t>Contact externe : Adresse Complément</t>
-  </si>
-  <si>
-    <t>contact.address_complement</t>
-  </si>
-  <si>
-    <t>[contact.address_complement]</t>
-  </si>
-  <si>
-    <t>Contact externe : Adresse Code Postal</t>
-  </si>
-  <si>
-    <t>contact.address_postal_code</t>
-  </si>
-  <si>
-    <t>[contact.address_postal_code]</t>
-  </si>
-  <si>
-    <t>Contact externe : Adresse Ville</t>
-  </si>
-  <si>
-    <t>contact.address_town</t>
-  </si>
-  <si>
-    <t>[contact.address_town]</t>
-  </si>
-  <si>
-    <t>Contact externe : Adresse Pays</t>
-  </si>
-  <si>
-    <t>contact.address_country</t>
-  </si>
-  <si>
-    <t>[contact.address_country]</t>
-  </si>
-  <si>
-    <t>Contact externe : Adresse Téléphone</t>
-  </si>
-  <si>
-    <t>contact.phone</t>
-  </si>
-  <si>
-    <t>[contact.phone]</t>
-  </si>
-  <si>
-    <t>Contact externe : Adresse Courriel</t>
-  </si>
-  <si>
-    <t>contact.email</t>
-  </si>
-  <si>
-    <t>[contact.email]</t>
-  </si>
-  <si>
-    <t>Contact externe : Adresse Site internet</t>
-  </si>
-  <si>
-    <t>contact.website</t>
-  </si>
-  <si>
-    <t>[contact.website]</t>
-  </si>
-  <si>
-    <t>Contact externe : Formule de politesse de début de courrier</t>
-  </si>
-  <si>
-    <t>contact.salutation_header</t>
-  </si>
-  <si>
-    <t>[contact.salutation_header]</t>
-  </si>
-  <si>
-    <t>Contact externe : Formule de politesse de fin de courrier</t>
-  </si>
-  <si>
-    <t>contact.salutation_footer</t>
-  </si>
-  <si>
-    <t>[contact.salutation_footer]</t>
-  </si>
-  <si>
-    <t>Contact interne: Nom</t>
-  </si>
-  <si>
-    <t>user.lastname</t>
-  </si>
-  <si>
-    <t>[user.lastname]</t>
-  </si>
-  <si>
-    <t>Contact interne: Prénom</t>
-  </si>
-  <si>
-    <t>user.firstname</t>
-  </si>
-  <si>
-    <t>[user.firstname]</t>
-  </si>
-  <si>
-    <t>Courrier : Service initiateur</t>
-  </si>
-  <si>
-    <t>res_letterbox.initiator</t>
-  </si>
-  <si>
-    <t>[res_letterbox.initiator]</t>
-  </si>
-  <si>
-    <t>Courrier: Service Traitant</t>
-  </si>
-  <si>
-    <t>res_letterbox.destination</t>
-  </si>
-  <si>
-    <t>[res_letterbox.destination]</t>
-  </si>
-  <si>
-    <t>Courrier: Type de document</t>
-  </si>
-  <si>
-    <t>res_letterbox.type_label</t>
-  </si>
-  <si>
-    <t>[res_letterbox.type_label]</t>
-  </si>
-  <si>
-    <t>Courrier: Catégorie</t>
-  </si>
-  <si>
-    <t>res_letterbox.category_id</t>
-  </si>
-  <si>
-    <t>[res_letterbox.category_id]</t>
-  </si>
-  <si>
-    <t>Courrier: Nature</t>
-  </si>
-  <si>
-    <t>res_letterbox.nature_id</t>
-  </si>
-  <si>
-    <t>[res_letterbox.nature_id]</t>
-  </si>
-  <si>
-    <t>Courrier: Date d'arrivée</t>
-  </si>
-  <si>
-    <t>res_letterbox.admission_date</t>
-  </si>
-  <si>
-    <t>[res_letterbox.admission_date]</t>
-  </si>
-  <si>
-    <t>Courrier: Date du courrier</t>
-  </si>
-  <si>
-    <t>res_letterbox.doc_date</t>
-  </si>
-  <si>
-    <t>[res_letterbox.doc_date]</t>
-  </si>
-  <si>
-    <t>Courrier: Date limite de traitement</t>
-  </si>
-  <si>
-    <t>res_letterbox.process_limit_date</t>
-  </si>
-  <si>
-    <t>[res_letterbox.process_limit_date]</t>
-  </si>
-  <si>
-    <t>Courrier: Notes de traitement</t>
-  </si>
-  <si>
-    <t>res_letterbox.process_notes</t>
-  </si>
-  <si>
-    <t>[res_letterbox.process_notes]</t>
-  </si>
-  <si>
-    <t>Courrier: Date de clôture</t>
-  </si>
-  <si>
-    <t>res_letterbox.closing_date</t>
-  </si>
-  <si>
-    <t>[res_letterbox.closing_date]</t>
-  </si>
-  <si>
-    <t>Courrier: Objet</t>
-  </si>
-  <si>
-    <t>res_letterbox.subject</t>
-  </si>
-  <si>
-    <t>[res_letterbox.subject]</t>
-  </si>
-  <si>
-    <t>Courrier: Numéro chrono entrant</t>
-  </si>
-  <si>
-    <t>res_letterbox.alt_identifier</t>
-  </si>
-  <si>
-    <t>[res_letterbox.alt_identifier]</t>
-  </si>
-  <si>
-    <t>Réponse : Numéro chrono de la réponse</t>
-  </si>
-  <si>
-    <t>attachments.chrono</t>
-  </si>
-  <si>
-    <t>[attachments.chrono]</t>
-  </si>
-  <si>
-    <t>Document: Auteur</t>
-  </si>
-  <si>
-    <t>res_letterbox.author</t>
-  </si>
-  <si>
-    <t>[res_letterbox.author]</t>
-  </si>
-  <si>
-    <t>Document: Date d'enregistrement</t>
-  </si>
-  <si>
-    <t>res_letterbox.creation_date</t>
-  </si>
-  <si>
-    <t>[res_letterbox.creation_date]</t>
-  </si>
-  <si>
-    <t>Special: Date du jour</t>
-  </si>
-  <si>
-    <t>datetime.date</t>
-  </si>
-  <si>
-    <t>[datetime.date]</t>
-  </si>
-  <si>
-    <t>Special: Nom du destinataire traitant</t>
-  </si>
-  <si>
-    <t>Special: Prénom du destinataire traitant</t>
-  </si>
-  <si>
-    <t>Special: Téléphone du destinataire traitant</t>
-  </si>
-  <si>
-    <t>user.phone</t>
-  </si>
-  <si>
-    <t>[user.phone]</t>
-  </si>
-  <si>
-    <t>Special: Mail du destinataire traitant</t>
-  </si>
-  <si>
-    <t>user.mail</t>
-  </si>
-  <si>
-    <t>[user.mail]</t>
-  </si>
-  <si>
-    <t>[attachments.chronoBarCode;ope=changepic]</t>
-  </si>
-  <si>
-    <t>Insérer une image juste au dessus de cette balise</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="153" uniqueCount="148">
+  <si>
+    <t xml:space="preserve">TITLE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TAG</t>
+  </si>
+  <si>
+    <t xml:space="preserve">VAR</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Contact externe : Type de contact</t>
+  </si>
+  <si>
+    <t xml:space="preserve">contact.contact_type_label</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[contact.contact_type_label]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Contact externe : Structure</t>
+  </si>
+  <si>
+    <t xml:space="preserve">contact.society</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[contact.society]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Contact externe : Sigle de la structure</t>
+  </si>
+  <si>
+    <t xml:space="preserve">contact.society_short</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[contact.society_short]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Contact externes : nom du contact</t>
+  </si>
+  <si>
+    <t xml:space="preserve">contact.contact_lastname</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[contact.contact_lastname]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Contact externes : prénom du contact</t>
+  </si>
+  <si>
+    <t xml:space="preserve">contact.contact_firstname</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[contact.contact_firstname]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Contact externe : Adresse Dénomination</t>
+  </si>
+  <si>
+    <t xml:space="preserve">contact.contact_purpose_label</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[contact.contact_purpose_label]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Contact externe : Adresse Service</t>
+  </si>
+  <si>
+    <t xml:space="preserve">contact.departement</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[contact.departement]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Contact externe : Adresse Civilité</t>
+  </si>
+  <si>
+    <t xml:space="preserve">contact.title</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[contact.title]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Contact externe : Adresse Nom</t>
+  </si>
+  <si>
+    <t xml:space="preserve">contact.lastname</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[contact.lastname]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Contact externe : Adresse Prénom</t>
+  </si>
+  <si>
+    <t xml:space="preserve">contact.firstname</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[contact.firstname]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Contact externe : Adresse Fonction</t>
+  </si>
+  <si>
+    <t xml:space="preserve">contact.function</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[contact.function]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Contact externe : Adresse Etage, bureau, porte</t>
+  </si>
+  <si>
+    <t xml:space="preserve">contact.occupancy</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[contact.occupancy]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Contact externe : Adresse N°</t>
+  </si>
+  <si>
+    <t xml:space="preserve">contact.address_num</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[contact.address_num]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Contact externe : Adresse Rue</t>
+  </si>
+  <si>
+    <t xml:space="preserve">contact.address_street</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[contact.address_street]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Contact externe : Adresse Complément</t>
+  </si>
+  <si>
+    <t xml:space="preserve">contact.address_complement</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[contact.address_complement]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Contact externe : Adresse Code Postal</t>
+  </si>
+  <si>
+    <t xml:space="preserve">contact.address_postal_code</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[contact.address_postal_code]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Contact externe : Adresse Ville</t>
+  </si>
+  <si>
+    <t xml:space="preserve">contact.address_town</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[contact.address_town]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Contact externe : Adresse Pays</t>
+  </si>
+  <si>
+    <t xml:space="preserve">contact.address_country</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[contact.address_country]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Contact externe : Adresse Téléphone</t>
+  </si>
+  <si>
+    <t xml:space="preserve">contact.phone</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[contact.phone]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Contact externe : Adresse Courriel</t>
+  </si>
+  <si>
+    <t xml:space="preserve">contact.email</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[contact.email]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Contact externe : Adresse Site internet</t>
+  </si>
+  <si>
+    <t xml:space="preserve">contact.website</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[contact.website]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Contact externe : Formule de politesse de début de courrier</t>
+  </si>
+  <si>
+    <t xml:space="preserve">contact.salutation_header</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[contact.salutation_header]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Contact externe : Formule de politesse de fin de courrier</t>
+  </si>
+  <si>
+    <t xml:space="preserve">contact.salutation_footer</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[contact.salutation_footer]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Contact interne: Nom</t>
+  </si>
+  <si>
+    <t xml:space="preserve">user.lastname</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[user.lastname]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Contact interne: Prénom</t>
+  </si>
+  <si>
+    <t xml:space="preserve">user.firstname</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[user.firstname]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Courrier : Service initiateur</t>
+  </si>
+  <si>
+    <t xml:space="preserve">res_letterbox.initiator</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[res_letterbox.initiator]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Courrier: Service Traitant</t>
+  </si>
+  <si>
+    <t xml:space="preserve">res_letterbox.destination</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[res_letterbox.destination]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Courrier: Type de document</t>
+  </si>
+  <si>
+    <t xml:space="preserve">res_letterbox.type_label</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[res_letterbox.type_label]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Courrier: Catégorie</t>
+  </si>
+  <si>
+    <t xml:space="preserve">res_letterbox.category_id</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[res_letterbox.category_id]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Courrier: Nature</t>
+  </si>
+  <si>
+    <t xml:space="preserve">res_letterbox.nature_id</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[res_letterbox.nature_id]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Courrier: Date d'arrivée</t>
+  </si>
+  <si>
+    <t xml:space="preserve">res_letterbox.admission_date</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[res_letterbox.admission_date]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Courrier: Date du courrier</t>
+  </si>
+  <si>
+    <t xml:space="preserve">res_letterbox.doc_date</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[res_letterbox.doc_date]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Courrier: Date limite de traitement</t>
+  </si>
+  <si>
+    <t xml:space="preserve">res_letterbox.process_limit_date</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[res_letterbox.process_limit_date]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Courrier: Notes de traitement</t>
+  </si>
+  <si>
+    <t xml:space="preserve">res_letterbox.process_notes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[res_letterbox.process_notes]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Courrier: Date de clôture</t>
+  </si>
+  <si>
+    <t xml:space="preserve">res_letterbox.closing_date</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[res_letterbox.closing_date]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Courrier: Objet</t>
+  </si>
+  <si>
+    <t xml:space="preserve">res_letterbox.subject</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[res_letterbox.subject]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Courrier: Numéro chrono entrant</t>
+  </si>
+  <si>
+    <t xml:space="preserve">res_letterbox.alt_identifier</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[res_letterbox.alt_identifier]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Réponse : Numéro chrono de la réponse</t>
+  </si>
+  <si>
+    <t xml:space="preserve">attachments.chrono</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[attachments.chrono]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Document: Auteur</t>
+  </si>
+  <si>
+    <t xml:space="preserve">res_letterbox.author</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[res_letterbox.author]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Document: Date d'enregistrement</t>
+  </si>
+  <si>
+    <t xml:space="preserve">res_letterbox.creation_date</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[res_letterbox.creation_date]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Special: Date du jour</t>
+  </si>
+  <si>
+    <t xml:space="preserve">datetime.date</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[datetime.date]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Special: Nom du destinataire traitant</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Special: Prénom du destinataire traitant</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Special: Téléphone du destinataire traitant</t>
+  </si>
+  <si>
+    <t xml:space="preserve">user.phone</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[user.phone]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Special: Mail du destinataire traitant</t>
+  </si>
+  <si>
+    <t xml:space="preserve">user.mail</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[user.mail]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[attachments.chronoBarCode;ope=changepic]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Insérer une image juste au dessus de cette balise</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Service initiateur: Identifiant de l'entité</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[res_letterbox.initiator_entity_id]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Service initiateur: Nom long de l'entité</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[res_letterbox.initiator_entity_label]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Service initiateur: Nom court de l'entité</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[res_letterbox.initiator_short_label]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Service initiateur: Email de l'entité</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[res_letterbox.initiator_email]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Service initiateur: Identifiant de l'entité parente</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[res_letterbox.initiator_parent_entity_id]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Service initiateur: Type de l'entité</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[res_letterbox.initiator_entity_type]</t>
   </si>
 </sst>
 </file>
@@ -432,9 +473,9 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="GENERAL"/>
+    <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="16">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -456,6 +497,87 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
+    </font>
+    <font>
+      <b val="true"/>
+      <sz val="24"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="18"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF333333"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <i val="true"/>
+      <sz val="10"/>
+      <color rgb="FF808080"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF006600"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF996600"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FFCC0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b val="true"/>
+      <sz val="10"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b val="true"/>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <b val="true"/>
@@ -466,7 +588,7 @@
       <charset val="1"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -475,12 +597,48 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor rgb="FFFFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFCCFFCC"/>
+        <bgColor rgb="FFCCFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCCCC"/>
+        <bgColor rgb="FFDDDDDD"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFCC0000"/>
+        <bgColor rgb="FF800000"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF000000"/>
+        <bgColor rgb="FF003300"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF808080"/>
+        <bgColor rgb="FF969696"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFDDDDDD"/>
-        <bgColor rgb="FFCCFFCC"/>
+        <bgColor rgb="FFFFCCCC"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border diagonalUp="false" diagonalDown="false">
       <left/>
       <right/>
@@ -488,8 +646,23 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left style="thin">
+        <color rgb="FF808080"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF808080"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF808080"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF808080"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="20">
+  <cellStyleXfs count="36">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -513,39 +686,107 @@
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="2" borderId="1" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="9" fillId="3" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="10" fillId="2" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="11" fillId="4" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="11" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="12" fillId="5" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="13" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="14" fillId="6" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="14" fillId="7" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="13" fillId="8" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="15" fillId="8" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="6">
+  <cellStyles count="22">
     <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
     <cellStyle name="Comma" xfId="15" builtinId="3" customBuiltin="false"/>
     <cellStyle name="Comma [0]" xfId="16" builtinId="6" customBuiltin="false"/>
     <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
     <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
     <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
+    <cellStyle name="Heading" xfId="20" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Heading 1" xfId="21" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Heading 2" xfId="22" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Text" xfId="23" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Note" xfId="24" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Footnote" xfId="25" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Status" xfId="26" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Good" xfId="27" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Neutral" xfId="28" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Bad" xfId="29" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Warning" xfId="30" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Error" xfId="31" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Accent" xfId="32" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Accent 1" xfId="33" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Accent 2" xfId="34" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Accent 3" xfId="35" builtinId="53" customBuiltin="true"/>
   </cellStyles>
   <colors>
     <indexedColors>
       <rgbColor rgb="FF000000"/>
       <rgbColor rgb="FFFFFFFF"/>
-      <rgbColor rgb="FFFF0000"/>
+      <rgbColor rgb="FFCC0000"/>
       <rgbColor rgb="FF00FF00"/>
       <rgbColor rgb="FF0000FF"/>
       <rgbColor rgb="FFFFFF00"/>
       <rgbColor rgb="FFFF00FF"/>
       <rgbColor rgb="FF00FFFF"/>
       <rgbColor rgb="FF800000"/>
-      <rgbColor rgb="FF008000"/>
+      <rgbColor rgb="FF006600"/>
       <rgbColor rgb="FF000080"/>
-      <rgbColor rgb="FF808000"/>
+      <rgbColor rgb="FF996600"/>
       <rgbColor rgb="FF800080"/>
       <rgbColor rgb="FF008080"/>
       <rgbColor rgb="FFC0C0C0"/>
@@ -573,7 +814,7 @@
       <rgbColor rgb="FF99CCFF"/>
       <rgbColor rgb="FFFF99CC"/>
       <rgbColor rgb="FFCC99FF"/>
-      <rgbColor rgb="FFFFCC99"/>
+      <rgbColor rgb="FFFFCCCC"/>
       <rgbColor rgb="FF3366FF"/>
       <rgbColor rgb="FF33CCCC"/>
       <rgbColor rgb="FF99CC00"/>
@@ -600,20 +841,20 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C48"/>
+  <dimension ref="A1:C55"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B23" activeCellId="0" sqref="B23"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A58" activeCellId="0" sqref="A58"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8"/>
+  <sheetFormatPr defaultRowHeight="13.8" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="43.4251012145749"/>
-    <col collapsed="false" hidden="false" max="3" min="2" style="0" width="33.7125506072874"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="10.5708502024292"/>
-    <col collapsed="false" hidden="false" max="6" min="5" style="0" width="8.85425101214575"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="31.1417004048583"/>
-    <col collapsed="false" hidden="false" max="1025" min="8" style="0" width="8.85425101214575"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="43.43"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="2" style="0" width="33.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="10.57"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="5" style="0" width="8.85"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="31.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="8" style="0" width="8.85"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1133,10 +1374,58 @@
         <v>135</v>
       </c>
     </row>
+    <row r="50" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A50" s="2" t="s">
+        <v>136</v>
+      </c>
+      <c r="C50" s="2" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="51" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A51" s="2" t="s">
+        <v>138</v>
+      </c>
+      <c r="C51" s="2" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="52" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A52" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="C52" s="2" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="53" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A53" s="2" t="s">
+        <v>142</v>
+      </c>
+      <c r="C53" s="2" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="54" customFormat="false" ht="25.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A54" s="2" t="s">
+        <v>144</v>
+      </c>
+      <c r="C54" s="2" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="55" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A55" s="2" t="s">
+        <v>146</v>
+      </c>
+      <c r="C55" s="2" t="s">
+        <v>147</v>
+      </c>
+    </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -1151,18 +1440,18 @@
   </sheetPr>
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.85425101214575"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="1" style="0" width="8.85"/>
   </cols>
   <sheetData/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -1177,18 +1466,18 @@
   </sheetPr>
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.85425101214575"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="1" style="0" width="8.85"/>
   </cols>
   <sheetData/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>

</xml_diff>

<commit_message>
FEAT template with contact.afnor
</commit_message>
<xml_diff>
--- a/modules/templates/templates/styles/office/spreadsheet.xlsx
+++ b/modules/templates/templates/styles/office/spreadsheet.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="153" uniqueCount="148">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="156" uniqueCount="151">
   <si>
     <t xml:space="preserve">TITLE</t>
   </si>
@@ -31,6 +31,15 @@
   </si>
   <si>
     <t xml:space="preserve">VAR</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Adresse selon la norme AFNOR NF Z10-011</t>
+  </si>
+  <si>
+    <t xml:space="preserve">contact.afnor</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[contact.afnor]</t>
   </si>
   <si>
     <t xml:space="preserve">Contact externe : Type de contact</t>
@@ -475,7 +484,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="16">
+  <fonts count="5">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -500,87 +509,6 @@
     </font>
     <font>
       <b val="true"/>
-      <sz val="24"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <sz val="18"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FF333333"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <i val="true"/>
-      <sz val="10"/>
-      <color rgb="FF808080"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FF006600"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FF996600"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FFCC0000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <b val="true"/>
-      <sz val="10"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <b val="true"/>
-      <sz val="10"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <b val="true"/>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
@@ -588,7 +516,7 @@
       <charset val="1"/>
     </font>
   </fonts>
-  <fills count="9">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -597,48 +525,12 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor rgb="FFFFFFFF"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFCCFFCC"/>
-        <bgColor rgb="FFCCFFFF"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCCCC"/>
-        <bgColor rgb="FFDDDDDD"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFCC0000"/>
-        <bgColor rgb="FF800000"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF000000"/>
-        <bgColor rgb="FF003300"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF808080"/>
-        <bgColor rgb="FF969696"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="FFDDDDDD"/>
-        <bgColor rgb="FFFFCCCC"/>
+        <bgColor rgb="FFCCFFCC"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="1">
     <border diagonalUp="false" diagonalDown="false">
       <left/>
       <right/>
@@ -646,23 +538,8 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border diagonalUp="false" diagonalDown="false">
-      <left style="thin">
-        <color rgb="FF808080"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF808080"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF808080"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF808080"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
-  <cellStyleXfs count="36">
+  <cellStyleXfs count="20">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -686,61 +563,17 @@
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="7" fillId="2" borderId="1" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="9" fillId="3" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="10" fillId="2" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="11" fillId="4" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="11" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="12" fillId="5" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="13" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="14" fillId="6" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="14" fillId="7" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="13" fillId="8" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="15" fillId="8" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -749,44 +582,28 @@
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
-  <cellStyles count="22">
+  <cellStyles count="6">
     <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
     <cellStyle name="Comma" xfId="15" builtinId="3" customBuiltin="false"/>
     <cellStyle name="Comma [0]" xfId="16" builtinId="6" customBuiltin="false"/>
     <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
     <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
     <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
-    <cellStyle name="Heading" xfId="20" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Heading 1" xfId="21" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Heading 2" xfId="22" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Text" xfId="23" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Note" xfId="24" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Footnote" xfId="25" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Status" xfId="26" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Good" xfId="27" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Neutral" xfId="28" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Bad" xfId="29" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Warning" xfId="30" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Error" xfId="31" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Accent" xfId="32" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Accent 1" xfId="33" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Accent 2" xfId="34" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Accent 3" xfId="35" builtinId="53" customBuiltin="true"/>
   </cellStyles>
   <colors>
     <indexedColors>
       <rgbColor rgb="FF000000"/>
       <rgbColor rgb="FFFFFFFF"/>
-      <rgbColor rgb="FFCC0000"/>
+      <rgbColor rgb="FFFF0000"/>
       <rgbColor rgb="FF00FF00"/>
       <rgbColor rgb="FF0000FF"/>
       <rgbColor rgb="FFFFFF00"/>
       <rgbColor rgb="FFFF00FF"/>
       <rgbColor rgb="FF00FFFF"/>
       <rgbColor rgb="FF800000"/>
-      <rgbColor rgb="FF006600"/>
+      <rgbColor rgb="FF008000"/>
       <rgbColor rgb="FF000080"/>
-      <rgbColor rgb="FF996600"/>
+      <rgbColor rgb="FF808000"/>
       <rgbColor rgb="FF800080"/>
       <rgbColor rgb="FF008080"/>
       <rgbColor rgb="FFC0C0C0"/>
@@ -814,7 +631,7 @@
       <rgbColor rgb="FF99CCFF"/>
       <rgbColor rgb="FFFF99CC"/>
       <rgbColor rgb="FFCC99FF"/>
-      <rgbColor rgb="FFFFCCCC"/>
+      <rgbColor rgb="FFFFCC99"/>
       <rgbColor rgb="FF3366FF"/>
       <rgbColor rgb="FF33CCCC"/>
       <rgbColor rgb="FF99CC00"/>
@@ -841,15 +658,15 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C55"/>
+  <dimension ref="A1:C56"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A58" activeCellId="0" sqref="A58"/>
+      <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="43.43"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="42.33"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="2" style="0" width="33.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="10.57"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="5" style="0" width="8.85"/>
@@ -869,13 +686,13 @@
       </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="s">
+      <c r="A2" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="0" t="s">
+      <c r="B2" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="0" t="s">
+      <c r="C2" s="2" t="s">
         <v>5</v>
       </c>
     </row>
@@ -1099,7 +916,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="23" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="0" t="s">
         <v>66</v>
       </c>
@@ -1121,7 +938,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="25" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A25" s="0" t="s">
         <v>72</v>
       </c>
@@ -1324,15 +1141,15 @@
         <v>126</v>
       </c>
       <c r="B43" s="0" t="s">
-        <v>73</v>
+        <v>127</v>
       </c>
       <c r="C43" s="0" t="s">
-        <v>74</v>
+        <v>128</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="0" t="s">
-        <v>127</v>
+        <v>129</v>
       </c>
       <c r="B44" s="0" t="s">
         <v>76</v>
@@ -1343,13 +1160,13 @@
     </row>
     <row r="45" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="0" t="s">
-        <v>128</v>
+        <v>130</v>
       </c>
       <c r="B45" s="0" t="s">
-        <v>129</v>
+        <v>79</v>
       </c>
       <c r="C45" s="0" t="s">
-        <v>130</v>
+        <v>80</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1363,63 +1180,74 @@
         <v>133</v>
       </c>
     </row>
-    <row r="48" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A48" s="0" t="s">
+    <row r="47" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A47" s="0" t="s">
         <v>134</v>
       </c>
-      <c r="B48" s="0" t="s">
+      <c r="B47" s="0" t="s">
         <v>135</v>
       </c>
-      <c r="C48" s="0" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="50" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A50" s="2" t="s">
+      <c r="C47" s="0" t="s">
         <v>136</v>
       </c>
-      <c r="C50" s="2" t="s">
+    </row>
+    <row r="49" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A49" s="0" t="s">
         <v>137</v>
       </c>
+      <c r="B49" s="0" t="s">
+        <v>138</v>
+      </c>
+      <c r="C49" s="0" t="s">
+        <v>138</v>
+      </c>
     </row>
     <row r="51" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A51" s="2" t="s">
-        <v>138</v>
-      </c>
-      <c r="C51" s="2" t="s">
+      <c r="A51" s="3" t="s">
         <v>139</v>
       </c>
+      <c r="C51" s="3" t="s">
+        <v>140</v>
+      </c>
     </row>
     <row r="52" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A52" s="2" t="s">
-        <v>140</v>
-      </c>
-      <c r="C52" s="2" t="s">
+      <c r="A52" s="3" t="s">
         <v>141</v>
       </c>
+      <c r="C52" s="3" t="s">
+        <v>142</v>
+      </c>
     </row>
     <row r="53" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A53" s="2" t="s">
-        <v>142</v>
-      </c>
-      <c r="C53" s="2" t="s">
+      <c r="A53" s="3" t="s">
         <v>143</v>
       </c>
-    </row>
-    <row r="54" customFormat="false" ht="25.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A54" s="2" t="s">
+      <c r="C53" s="3" t="s">
         <v>144</v>
       </c>
-      <c r="C54" s="2" t="s">
+    </row>
+    <row r="54" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A54" s="3" t="s">
         <v>145</v>
       </c>
-    </row>
-    <row r="55" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A55" s="2" t="s">
+      <c r="C54" s="3" t="s">
         <v>146</v>
       </c>
-      <c r="C55" s="2" t="s">
+    </row>
+    <row r="55" customFormat="false" ht="25.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A55" s="3" t="s">
         <v>147</v>
+      </c>
+      <c r="C55" s="3" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="56" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A56" s="3" t="s">
+        <v>149</v>
+      </c>
+      <c r="C56" s="3" t="s">
+        <v>150</v>
       </c>
     </row>
   </sheetData>
@@ -1444,7 +1272,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="1" style="0" width="8.85"/>
   </cols>
@@ -1470,7 +1298,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="1" style="0" width="8.85"/>
   </cols>

</xml_diff>

<commit_message>
FEAT #7647 change to contact.postal_address in templates
</commit_message>
<xml_diff>
--- a/modules/templates/templates/styles/office/spreadsheet.xlsx
+++ b/modules/templates/templates/styles/office/spreadsheet.xlsx
@@ -36,10 +36,10 @@
     <t xml:space="preserve">Adresse selon la norme AFNOR NF Z10-011</t>
   </si>
   <si>
-    <t xml:space="preserve">contact.afnor</t>
-  </si>
-  <si>
-    <t xml:space="preserve">[contact.afnor]</t>
+    <t xml:space="preserve">contact.postal_address</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[contact.postal_address]</t>
   </si>
   <si>
     <t xml:space="preserve">Contact externe : Type de contact</t>
@@ -661,7 +661,7 @@
   <dimension ref="A1:C56"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
+      <selection pane="topLeft" activeCell="C14" activeCellId="0" sqref="C13:C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1269,7 +1269,7 @@
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="C13:C14 A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1295,7 +1295,7 @@
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="C13:C14 A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>